<commit_message>
Add input file for Developer
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/07-long-term-planning-DEV.xlsx
+++ b/ampl-data-input-excel/07-long-term-planning-DEV.xlsx
@@ -42,13 +42,13 @@
     <t xml:space="preserve">Alojzy</t>
   </si>
   <si>
-    <t xml:space="preserve">p2.m main task</t>
+    <t xml:space="preserve">Main tasks p2.*</t>
   </si>
   <si>
     <t xml:space="preserve">Bartłomiej</t>
   </si>
   <si>
-    <t xml:space="preserve">p3.m main task</t>
+    <t xml:space="preserve">Main tasks p3.*</t>
   </si>
   <si>
     <t xml:space="preserve">Franciszek</t>
@@ -60,13 +60,13 @@
     <t xml:space="preserve">Paweł</t>
   </si>
   <si>
-    <t xml:space="preserve">p4.m main task</t>
+    <t xml:space="preserve">Main tasks p4.*</t>
   </si>
   <si>
     <t xml:space="preserve">Wojciech</t>
   </si>
   <si>
-    <t xml:space="preserve">P5.m main task</t>
+    <t xml:space="preserve">Main tasks p5.*</t>
   </si>
   <si>
     <t xml:space="preserve">Start day</t>
@@ -282,7 +282,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -316,11 +316,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -383,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -394,10 +389,6 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -674,7 +665,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,7 +694,7 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -711,7 +702,7 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -719,7 +710,7 @@
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -727,7 +718,7 @@
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -756,21 +747,21 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="23" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -838,16 +829,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14" t="n">
+      <c r="A2" s="13" t="n">
         <v>45651</v>
       </c>
     </row>
@@ -875,57 +866,57 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="4" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="4" width="19.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="19.48"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="3" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="3" t="n">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E2" s="19" t="n">
+      <c r="E2" s="18" t="n">
         <v>45840</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="19" t="n">
+      <c r="G2" s="18" t="n">
         <v>45840</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -957,230 +948,230 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="10" t="n">
+      <c r="D2" s="9" t="n">
         <v>670</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="10" t="n">
+      <c r="D3" s="9" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="11" t="n">
+      <c r="B4" s="10" t="n">
         <v>45778</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="10" t="n">
         <v>45790</v>
       </c>
-      <c r="D4" s="10" t="n">
+      <c r="D4" s="9" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="10" t="n">
+      <c r="D5" s="9" t="n">
         <v>636</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="11" t="n">
+      <c r="B6" s="10" t="n">
         <v>45808</v>
       </c>
-      <c r="C6" s="11" t="n">
+      <c r="C6" s="10" t="n">
         <v>45835</v>
       </c>
-      <c r="D6" s="10" t="n">
+      <c r="D6" s="9" t="n">
         <v>96</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="11" t="n">
+      <c r="B7" s="10" t="n">
         <v>45836</v>
       </c>
-      <c r="C7" s="11" t="n">
+      <c r="C7" s="10" t="n">
         <v>45849</v>
       </c>
-      <c r="D7" s="10" t="n">
+      <c r="D7" s="9" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="10" t="n">
+      <c r="D8" s="9" t="n">
         <v>1130</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="10" t="n">
+      <c r="D9" s="9" t="n">
         <v>160</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="11" t="n">
+      <c r="B10" s="10" t="n">
         <v>45857</v>
       </c>
-      <c r="C10" s="11" t="n">
+      <c r="C10" s="10" t="n">
         <v>45872</v>
       </c>
-      <c r="D10" s="10" t="n">
+      <c r="D10" s="9" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="10" t="n">
+      <c r="D11" s="9" t="n">
         <v>680</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="10" t="n">
+      <c r="D12" s="9" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="11" t="n">
+      <c r="B13" s="10" t="n">
         <v>45818</v>
       </c>
-      <c r="C13" s="11" t="n">
+      <c r="C13" s="10" t="n">
         <v>45831</v>
       </c>
-      <c r="D13" s="10" t="n">
+      <c r="D13" s="9" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="10" t="n">
+      <c r="D14" s="9" t="n">
         <v>1130</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="10" t="n">
+      <c r="D15" s="9" t="n">
         <v>160</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="11" t="n">
+      <c r="B16" s="10" t="n">
         <v>45899</v>
       </c>
-      <c r="C16" s="11" t="n">
+      <c r="C16" s="10" t="n">
         <v>45912</v>
       </c>
-      <c r="D16" s="10" t="n">
+      <c r="D16" s="9" t="n">
         <v>64</v>
       </c>
     </row>
@@ -1216,31 +1207,31 @@
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1269,26 +1260,26 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1317,34 +1308,34 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1373,34 +1364,34 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1430,86 +1421,86 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="13" t="n">
+      <c r="E2" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="F2" s="13" t="n">
+      <c r="F2" s="12" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="13" t="n">
+      <c r="E3" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="F3" s="13" t="n">
+      <c r="F3" s="12" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="11" t="n">
+      <c r="C4" s="10" t="n">
         <v>45778</v>
       </c>
-      <c r="D4" s="11" t="n">
+      <c r="D4" s="10" t="n">
         <v>45790</v>
       </c>
-      <c r="E4" s="13" t="n">
+      <c r="E4" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="12" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1520,16 +1511,16 @@
       <c r="B5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1540,16 +1531,16 @@
       <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="14" t="n">
+      <c r="C6" s="13" t="n">
         <v>45808</v>
       </c>
-      <c r="D6" s="14" t="n">
+      <c r="D6" s="13" t="n">
         <v>45835</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1560,76 +1551,76 @@
       <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="14" t="n">
+      <c r="C7" s="13" t="n">
         <v>45836</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="13" t="n">
         <v>45849</v>
       </c>
-      <c r="E7" s="4" t="n">
+      <c r="E7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="13" t="n">
+      <c r="E8" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="12" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="13" t="n">
+      <c r="E9" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="13" t="n">
+      <c r="F9" s="12" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="11" t="n">
+      <c r="C10" s="10" t="n">
         <v>45857</v>
       </c>
-      <c r="D10" s="11" t="n">
+      <c r="D10" s="10" t="n">
         <v>45872</v>
       </c>
-      <c r="E10" s="13" t="n">
+      <c r="E10" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="F10" s="13" t="n">
+      <c r="F10" s="12" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1640,16 +1631,16 @@
       <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="4" t="n">
+      <c r="E11" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1660,16 +1651,16 @@
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="4" t="n">
+      <c r="E12" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="3" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1680,96 +1671,96 @@
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="14" t="n">
+      <c r="C13" s="13" t="n">
         <v>45818</v>
       </c>
-      <c r="D13" s="14" t="n">
+      <c r="D13" s="13" t="n">
         <v>45831</v>
       </c>
-      <c r="E13" s="15" t="n">
+      <c r="E13" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="17" t="n">
+      <c r="E14" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="17" t="n">
+      <c r="F14" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="17" t="n">
+      <c r="E15" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="17" t="n">
+      <c r="F15" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="17" t="n">
+      <c r="E16" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="17" t="n">
+      <c r="F16" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="17" t="n">
+      <c r="E17" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="17" t="n">
+      <c r="F17" s="16" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1780,16 +1771,16 @@
       <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="15" t="n">
+      <c r="E18" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1800,16 +1791,16 @@
       <c r="B19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="15" t="n">
+      <c r="E19" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="3" t="n">
         <v>8</v>
       </c>
     </row>
@@ -1820,168 +1811,168 @@
       <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="14" t="n">
+      <c r="C20" s="13" t="n">
         <v>45899</v>
       </c>
-      <c r="D20" s="14" t="n">
+      <c r="D20" s="13" t="n">
         <v>45912</v>
       </c>
-      <c r="E20" s="15" t="n">
+      <c r="E20" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="18" t="n">
+      <c r="E21" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="F21" s="17" t="n">
+      <c r="F21" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="18" t="n">
+      <c r="E22" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="F22" s="17" t="n">
+      <c r="F22" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="18" t="n">
+      <c r="E23" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="F23" s="17" t="n">
+      <c r="F23" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="C24" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="18" t="n">
+      <c r="E24" s="17" t="n">
         <v>0</v>
       </c>
-      <c r="F24" s="17" t="n">
+      <c r="F24" s="16" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
@@ -2167,7 +2158,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -2175,19 +2166,19 @@
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2561,60 +2552,60 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
@@ -3026,7 +3017,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="3" width="11.53"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -3034,19 +3025,19 @@
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -3420,177 +3411,177 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3617,72 +3608,72 @@
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="4" width="11.53"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="3" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="22" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>